<commit_message>
Added Lastenheft - Jonas
</commit_message>
<xml_diff>
--- a/Anforderungsliste.xlsx
+++ b/Anforderungsliste.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CF9FE1-1C8D-4BBA-A82E-CD7196FA9197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2A8D3A-6EA3-4012-9661-3CB36FC9781F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -510,17 +510,17 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="50.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -532,7 +532,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -549,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -564,7 +564,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -579,7 +579,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -594,7 +594,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -609,7 +609,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -624,7 +624,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -639,7 +639,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -654,7 +654,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -669,7 +669,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -684,7 +684,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -699,7 +699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -714,7 +714,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -729,7 +729,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -744,7 +744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -759,7 +759,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -774,7 +774,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -789,7 +789,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -804,7 +804,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -819,7 +819,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -834,29 +834,29 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E26" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
word und pdf updated
</commit_message>
<xml_diff>
--- a/Anforderungsliste.xlsx
+++ b/Anforderungsliste.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BDA0C0-A0EA-4D75-8386-2CAD8BFCB595}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -129,7 +130,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,11 +243,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -519,18 +520,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +548,10 @@
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -825,17 +826,17 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>